<commit_message>
modificación y simplificacion de archivos
</commit_message>
<xml_diff>
--- a/EDA_Analisis_Mejores_Empresas_SP500/src/data/detalle_acciones_SP500.xlsx
+++ b/EDA_Analisis_Mejores_Empresas_SP500/src/data/detalle_acciones_SP500.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,143 +434,161 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Acción</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Rentabilidad Anual (%)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Volatilidad Anual</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Ratio de Sharpe</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Beta</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Apple</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>35.72</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>0.22</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>1.44</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.95</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Microsoft</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>14.56</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>0.2</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.53</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>1.19</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Nvidia</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>180.02</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>0.53</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>3.32</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>2.66</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Amazon</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>46.55</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>0.28</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>1.52</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>1.54</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Meta</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>70.08</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>0.36</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>1.84</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>1.55</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>S&amp;P 500</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>25.02</v>
-      </c>
       <c r="C7" t="n">
-        <v>14.53</v>
+        <v>24.12</v>
       </c>
       <c r="D7" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+        <v>0.13</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>